<commit_message>
Atualização dos atributos dos times.
</commit_message>
<xml_diff>
--- a/brasileirao/src/arquivos/partidas.xlsx
+++ b/brasileirao/src/arquivos/partidas.xlsx
@@ -194,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -277,361 +277,15 @@
     <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="193">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="143">
     <dxf>
       <font>
         <b/>
@@ -1911,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="H208" sqref="H208"/>
+    <sheetView tabSelected="1" topLeftCell="A203" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G220" sqref="G220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12429,10 +12083,10 @@
       <c r="B211" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C211" s="17">
-        <v>0</v>
-      </c>
-      <c r="D211" s="18">
+      <c r="C211" s="16">
+        <v>1</v>
+      </c>
+      <c r="D211" s="26">
         <v>0</v>
       </c>
       <c r="E211" s="8" t="s">
@@ -12441,8 +12095,8 @@
       <c r="F211" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G211" s="22">
-        <v>1000</v>
+      <c r="G211" s="24">
+        <v>200</v>
       </c>
       <c r="H211" s="22">
         <v>1000</v>
@@ -12479,10 +12133,10 @@
       <c r="B212" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C212" s="17">
-        <v>0</v>
-      </c>
-      <c r="D212" s="18">
+      <c r="C212" s="16">
+        <v>5</v>
+      </c>
+      <c r="D212" s="26">
         <v>0</v>
       </c>
       <c r="E212" s="10" t="s">
@@ -12491,20 +12145,20 @@
       <c r="F212" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G212" s="22">
-        <v>1000</v>
-      </c>
-      <c r="H212" s="22">
-        <v>1000</v>
-      </c>
-      <c r="I212" s="22">
-        <v>1000</v>
-      </c>
-      <c r="J212" s="22">
-        <v>1000</v>
-      </c>
-      <c r="K212" s="22">
-        <v>1000</v>
+      <c r="G212" s="24">
+        <v>200</v>
+      </c>
+      <c r="H212" s="24">
+        <v>200</v>
+      </c>
+      <c r="I212" s="24">
+        <v>200</v>
+      </c>
+      <c r="J212" s="24">
+        <v>200</v>
+      </c>
+      <c r="K212" s="24">
+        <v>200</v>
       </c>
       <c r="L212" s="22">
         <v>1000</v>
@@ -12529,10 +12183,10 @@
       <c r="B213" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C213" s="17">
-        <v>0</v>
-      </c>
-      <c r="D213" s="18">
+      <c r="C213" s="16">
+        <v>3</v>
+      </c>
+      <c r="D213" s="26">
         <v>0</v>
       </c>
       <c r="E213" s="8" t="s">
@@ -12541,14 +12195,14 @@
       <c r="F213" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G213" s="22">
-        <v>1000</v>
-      </c>
-      <c r="H213" s="22">
-        <v>1000</v>
-      </c>
-      <c r="I213" s="22">
-        <v>1000</v>
+      <c r="G213" s="24">
+        <v>200</v>
+      </c>
+      <c r="H213" s="24">
+        <v>200</v>
+      </c>
+      <c r="I213" s="24">
+        <v>200</v>
       </c>
       <c r="J213" s="22">
         <v>1000</v>
@@ -12579,11 +12233,11 @@
       <c r="B214" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C214" s="17">
-        <v>0</v>
-      </c>
-      <c r="D214" s="18">
-        <v>0</v>
+      <c r="C214" s="16">
+        <v>0</v>
+      </c>
+      <c r="D214" s="26">
+        <v>1</v>
       </c>
       <c r="E214" s="10" t="s">
         <v>0</v>
@@ -12591,8 +12245,8 @@
       <c r="F214" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G214" s="22">
-        <v>1000</v>
+      <c r="G214" s="24">
+        <v>200</v>
       </c>
       <c r="H214" s="22">
         <v>1000</v>
@@ -12629,10 +12283,10 @@
       <c r="B215" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C215" s="17">
-        <v>0</v>
-      </c>
-      <c r="D215" s="18">
+      <c r="C215" s="16">
+        <v>0</v>
+      </c>
+      <c r="D215" s="26">
         <v>0</v>
       </c>
       <c r="E215" s="8" t="s">
@@ -12679,10 +12333,10 @@
       <c r="B216" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C216" s="17">
-        <v>0</v>
-      </c>
-      <c r="D216" s="18">
+      <c r="C216" s="16">
+        <v>3</v>
+      </c>
+      <c r="D216" s="26">
         <v>0</v>
       </c>
       <c r="E216" s="10" t="s">
@@ -12691,14 +12345,14 @@
       <c r="F216" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G216" s="22">
-        <v>1000</v>
-      </c>
-      <c r="H216" s="22">
-        <v>1000</v>
-      </c>
-      <c r="I216" s="22">
-        <v>1000</v>
+      <c r="G216" s="24">
+        <v>200</v>
+      </c>
+      <c r="H216" s="24">
+        <v>200</v>
+      </c>
+      <c r="I216" s="24">
+        <v>200</v>
       </c>
       <c r="J216" s="22">
         <v>1000</v>
@@ -12729,11 +12383,11 @@
       <c r="B217" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C217" s="17">
-        <v>0</v>
-      </c>
-      <c r="D217" s="18">
-        <v>0</v>
+      <c r="C217" s="16">
+        <v>0</v>
+      </c>
+      <c r="D217" s="26">
+        <v>1</v>
       </c>
       <c r="E217" s="8" t="s">
         <v>6</v>
@@ -12741,8 +12395,8 @@
       <c r="F217" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G217" s="22">
-        <v>1000</v>
+      <c r="G217" s="24">
+        <v>200</v>
       </c>
       <c r="H217" s="22">
         <v>1000</v>
@@ -12779,11 +12433,11 @@
       <c r="B218" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C218" s="17">
-        <v>0</v>
-      </c>
-      <c r="D218" s="18">
-        <v>0</v>
+      <c r="C218" s="16">
+        <v>1</v>
+      </c>
+      <c r="D218" s="26">
+        <v>1</v>
       </c>
       <c r="E218" s="10" t="s">
         <v>8</v>
@@ -12791,11 +12445,11 @@
       <c r="F218" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G218" s="22">
-        <v>1000</v>
-      </c>
-      <c r="H218" s="22">
-        <v>1000</v>
+      <c r="G218" s="24">
+        <v>200</v>
+      </c>
+      <c r="H218" s="24">
+        <v>200</v>
       </c>
       <c r="I218" s="22">
         <v>1000</v>
@@ -12829,10 +12483,10 @@
       <c r="B219" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C219" s="17">
-        <v>0</v>
-      </c>
-      <c r="D219" s="18">
+      <c r="C219" s="16">
+        <v>1</v>
+      </c>
+      <c r="D219" s="26">
         <v>0</v>
       </c>
       <c r="E219" s="8" t="s">
@@ -12841,8 +12495,8 @@
       <c r="F219" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G219" s="22">
-        <v>1000</v>
+      <c r="G219" s="24">
+        <v>200</v>
       </c>
       <c r="H219" s="22">
         <v>1000</v>
@@ -12879,11 +12533,11 @@
       <c r="B220" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C220" s="17">
-        <v>0</v>
-      </c>
-      <c r="D220" s="18">
-        <v>0</v>
+      <c r="C220" s="16">
+        <v>0</v>
+      </c>
+      <c r="D220" s="26">
+        <v>1</v>
       </c>
       <c r="E220" s="10" t="s">
         <v>1</v>
@@ -12891,8 +12545,8 @@
       <c r="F220" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G220" s="22">
-        <v>1000</v>
+      <c r="G220" s="24">
+        <v>200</v>
       </c>
       <c r="H220" s="22">
         <v>1000</v>
@@ -20924,616 +20578,661 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B380">
-    <cfRule type="cellIs" dxfId="192" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="239" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F380">
-    <cfRule type="cellIs" dxfId="191" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="237" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E380">
-    <cfRule type="cellIs" dxfId="190" priority="227" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="236" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:P1">
-    <cfRule type="cellIs" dxfId="189" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="235" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:J3">
-    <cfRule type="cellIs" dxfId="188" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="234" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:P20">
-    <cfRule type="cellIs" dxfId="187" priority="223" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="232" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21:P30">
-    <cfRule type="cellIs" dxfId="186" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="231" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:P30">
-    <cfRule type="cellIs" dxfId="185" priority="221" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="230" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:K4">
-    <cfRule type="cellIs" dxfId="184" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="176" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:J5">
-    <cfRule type="cellIs" dxfId="183" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="175" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:P2">
-    <cfRule type="cellIs" dxfId="182" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="122" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:P3">
-    <cfRule type="cellIs" dxfId="181" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="121" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:P4">
-    <cfRule type="cellIs" dxfId="180" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="120" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:P5">
-    <cfRule type="cellIs" dxfId="179" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="119" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:P10">
-    <cfRule type="cellIs" dxfId="178" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="118" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:P40">
-    <cfRule type="cellIs" dxfId="177" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="117" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41:P50">
-    <cfRule type="cellIs" dxfId="176" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="116" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:P50">
-    <cfRule type="cellIs" dxfId="175" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="115" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51:P60">
-    <cfRule type="cellIs" dxfId="174" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="114" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G61:P70">
-    <cfRule type="cellIs" dxfId="173" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="113" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62:P70">
-    <cfRule type="cellIs" dxfId="172" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="112" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G71:P80">
-    <cfRule type="cellIs" dxfId="171" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="111" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81:P90">
-    <cfRule type="cellIs" dxfId="170" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="110" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82:P90">
-    <cfRule type="cellIs" dxfId="169" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="109" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91:P100">
-    <cfRule type="cellIs" dxfId="168" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="108" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G101:P110">
-    <cfRule type="cellIs" dxfId="167" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="107" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102:P110">
-    <cfRule type="cellIs" dxfId="166" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="106" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G111:P120">
-    <cfRule type="cellIs" dxfId="165" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="105" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G121:P130">
-    <cfRule type="cellIs" dxfId="164" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="104" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G122:P130">
-    <cfRule type="cellIs" dxfId="163" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="103" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G131:P140">
-    <cfRule type="cellIs" dxfId="162" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="102" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G141:P150">
-    <cfRule type="cellIs" dxfId="161" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="101" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G142:P150">
-    <cfRule type="cellIs" dxfId="160" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="100" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G151:P160">
-    <cfRule type="cellIs" dxfId="159" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="99" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G161:P170">
-    <cfRule type="cellIs" dxfId="158" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="98" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G162:P170">
-    <cfRule type="cellIs" dxfId="157" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="97" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L180:P180 H171:P171 K172:P172 J173:P173 K174:P174 I175:P175 M176:P176 H177:P177 L178:P178 I179:P179">
-    <cfRule type="cellIs" dxfId="156" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="96" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:P187 J181:P182 M183:P183 J184:P184 I185:P185 H186:P186 H190:P190 H188:P188 J189:P189">
-    <cfRule type="cellIs" dxfId="155" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="95" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:P187 J182:P182 M183:P183 J184:P184 I185:P185 H186:P186 H190:P190 H188:P188 J189:P189">
-    <cfRule type="cellIs" dxfId="154" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="94" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K191:P191 L192:P192 H193:P194 K195:P195 J196:P197 H198:P200">
-    <cfRule type="cellIs" dxfId="153" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="93" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J210:P210 L201:P201 H202:P203 J204:P204 I205:P205 H206:P206 J207:P208 I209:P209">
-    <cfRule type="cellIs" dxfId="152" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="92" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J210:P210 H202:P203 J204:P204 I205:P205 H206:P206 J207:P208 I209:P209">
-    <cfRule type="cellIs" dxfId="151" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="91" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G211:P220">
-    <cfRule type="cellIs" dxfId="150" priority="81" operator="equal">
+  <conditionalFormatting sqref="G215:P215 H211:P211 L212:P212 J213:P213 H214:P214 J216:P216 H217:P217 I218:P218 H219:P220">
+    <cfRule type="cellIs" dxfId="100" priority="90" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G221:P230">
-    <cfRule type="cellIs" dxfId="149" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="89" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G222:P230">
-    <cfRule type="cellIs" dxfId="148" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="88" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G231:P240">
-    <cfRule type="cellIs" dxfId="147" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="87" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G241:P250">
-    <cfRule type="cellIs" dxfId="146" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="86" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G242:P250">
-    <cfRule type="cellIs" dxfId="145" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="85" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G251:P260">
-    <cfRule type="cellIs" dxfId="144" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="84" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G261:P270">
-    <cfRule type="cellIs" dxfId="143" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="83" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G262:P270">
-    <cfRule type="cellIs" dxfId="142" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="82" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G271:P280">
-    <cfRule type="cellIs" dxfId="141" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="81" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G281:P290">
-    <cfRule type="cellIs" dxfId="140" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="80" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G282:P290">
-    <cfRule type="cellIs" dxfId="139" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="79" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G291:P300">
-    <cfRule type="cellIs" dxfId="138" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="78" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G301:P310">
-    <cfRule type="cellIs" dxfId="137" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="77" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G302:P310">
-    <cfRule type="cellIs" dxfId="136" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="76" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G311:P320">
-    <cfRule type="cellIs" dxfId="135" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="75" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G321:P330">
-    <cfRule type="cellIs" dxfId="134" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="74" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G322:P330">
-    <cfRule type="cellIs" dxfId="133" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="73" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G331:P340">
-    <cfRule type="cellIs" dxfId="132" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="72" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G341:P350">
-    <cfRule type="cellIs" dxfId="131" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="71" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G342:P350">
-    <cfRule type="cellIs" dxfId="130" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="70" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G351:P360">
-    <cfRule type="cellIs" dxfId="129" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="69" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G361:P370">
-    <cfRule type="cellIs" dxfId="128" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="68" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G362:P370">
-    <cfRule type="cellIs" dxfId="127" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="67" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G371:P380">
-    <cfRule type="cellIs" dxfId="126" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="66" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G171">
-    <cfRule type="cellIs" dxfId="111" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="65" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G172:J172">
-    <cfRule type="cellIs" dxfId="109" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="64" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G173:I173">
-    <cfRule type="cellIs" dxfId="107" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="63" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G174:J174">
-    <cfRule type="cellIs" dxfId="105" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="62" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G175:H175">
-    <cfRule type="cellIs" dxfId="103" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="61" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G176:L176">
-    <cfRule type="cellIs" dxfId="101" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="60" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G177">
-    <cfRule type="cellIs" dxfId="99" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="59" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G178:K178">
-    <cfRule type="cellIs" dxfId="97" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="58" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G179:H179">
-    <cfRule type="cellIs" dxfId="95" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="57" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G180:K180">
-    <cfRule type="cellIs" dxfId="93" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="56" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G181:I181">
-    <cfRule type="cellIs" dxfId="91" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="55" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G181:I181">
-    <cfRule type="cellIs" dxfId="89" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="54" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G182:I182">
-    <cfRule type="cellIs" dxfId="87" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="53" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G182:I182">
-    <cfRule type="cellIs" dxfId="85" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="52" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G183:L183">
-    <cfRule type="cellIs" dxfId="83" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="51" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G183:L183">
-    <cfRule type="cellIs" dxfId="81" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="50" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G184:I184">
-    <cfRule type="cellIs" dxfId="79" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="49" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G184:I184">
-    <cfRule type="cellIs" dxfId="77" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="48" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:H185">
-    <cfRule type="cellIs" dxfId="75" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="47" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:H185">
-    <cfRule type="cellIs" dxfId="73" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="46" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G186">
-    <cfRule type="cellIs" dxfId="71" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="45" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G186">
-    <cfRule type="cellIs" dxfId="69" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="44" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188">
-    <cfRule type="cellIs" dxfId="67" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="43" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188">
-    <cfRule type="cellIs" dxfId="65" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="42" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G189:I189">
-    <cfRule type="cellIs" dxfId="63" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="41" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G189:I189">
-    <cfRule type="cellIs" dxfId="61" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="40" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190">
-    <cfRule type="cellIs" dxfId="59" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="39" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190">
-    <cfRule type="cellIs" dxfId="57" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="38" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G191:J191">
-    <cfRule type="cellIs" dxfId="55" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G192:K192">
-    <cfRule type="cellIs" dxfId="53" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="36" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G193:G194">
-    <cfRule type="cellIs" dxfId="51" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="35" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G195:J195">
-    <cfRule type="cellIs" dxfId="49" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="34" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G196:I196">
-    <cfRule type="cellIs" dxfId="47" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G197:I197">
-    <cfRule type="cellIs" dxfId="45" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="32" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G198">
-    <cfRule type="cellIs" dxfId="43" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="31" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G199:G200">
-    <cfRule type="cellIs" dxfId="41" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:K201">
-    <cfRule type="cellIs" dxfId="39" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:K201">
-    <cfRule type="cellIs" dxfId="37" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="28" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202">
-    <cfRule type="cellIs" dxfId="35" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="27" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202">
-    <cfRule type="cellIs" dxfId="33" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="26" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203">
-    <cfRule type="cellIs" dxfId="31" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203">
-    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G204:I204">
-    <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G204:I204">
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G205:H205">
-    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G205:H205">
+    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G206">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G206">
+    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G207:I207">
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G207:I207">
+    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G208:I208">
+    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G208:I208">
+    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G209:H209">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G209:H209">
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+      <formula>$J$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G210:I210">
     <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G206">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+  <conditionalFormatting sqref="G210:I210">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G206">
+  <conditionalFormatting sqref="G211">
     <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G207:I207">
+  <conditionalFormatting sqref="G212:K212">
     <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G207:I207">
+  <conditionalFormatting sqref="G213:I213">
     <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G208:I208">
+  <conditionalFormatting sqref="G214">
     <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G208:I208">
+  <conditionalFormatting sqref="G216:I216">
     <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G209:H209">
+  <conditionalFormatting sqref="G217">
     <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G209:H209">
+  <conditionalFormatting sqref="G218:H218">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G210:I210">
+  <conditionalFormatting sqref="G219">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G210:I210">
+  <conditionalFormatting sqref="G220">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$J$4</formula>
     </cfRule>

</xml_diff>

<commit_message>
Métodos de atualizar classificação e artilharia funcionando.
</commit_message>
<xml_diff>
--- a/brasileirao/src/arquivos/partidas.xlsx
+++ b/brasileirao/src/arquivos/partidas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8115" yWindow="705" windowWidth="14220" windowHeight="13695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Rodadas" sheetId="2" r:id="rId1"/>
@@ -96,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,12 +127,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -194,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -271,12 +265,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
@@ -285,77 +273,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="143">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="133">
     <dxf>
       <font>
         <b/>
@@ -1565,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G220" sqref="G220"/>
+    <sheetView tabSelected="1" topLeftCell="A204" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F211" sqref="F211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9145,14 +9063,14 @@
       <c r="F152" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G152" s="24">
-        <v>200</v>
-      </c>
-      <c r="H152" s="24">
-        <v>200</v>
-      </c>
-      <c r="I152" s="24">
-        <v>200</v>
+      <c r="G152" s="22">
+        <v>18</v>
+      </c>
+      <c r="H152" s="22">
+        <v>19</v>
+      </c>
+      <c r="I152" s="22">
+        <v>148</v>
       </c>
       <c r="J152" s="22">
         <v>1000</v>
@@ -9195,17 +9113,17 @@
       <c r="F153" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G153" s="24">
-        <v>200</v>
-      </c>
-      <c r="H153" s="24">
-        <v>200</v>
-      </c>
-      <c r="I153" s="24">
-        <v>200</v>
-      </c>
-      <c r="J153" s="24">
-        <v>200</v>
+      <c r="G153" s="22">
+        <v>170</v>
+      </c>
+      <c r="H153" s="22">
+        <v>171</v>
+      </c>
+      <c r="I153" s="22">
+        <v>172</v>
+      </c>
+      <c r="J153" s="22">
+        <v>173</v>
       </c>
       <c r="K153" s="22">
         <v>1000</v>
@@ -9245,8 +9163,8 @@
       <c r="F154" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G154" s="24">
-        <v>200</v>
+      <c r="G154" s="22">
+        <v>164</v>
       </c>
       <c r="H154" s="22">
         <v>1000</v>
@@ -9295,8 +9213,8 @@
       <c r="F155" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G155" s="24">
-        <v>200</v>
+      <c r="G155" s="22">
+        <v>129</v>
       </c>
       <c r="H155" s="22">
         <v>1000</v>
@@ -9345,8 +9263,8 @@
       <c r="F156" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G156" s="24">
-        <v>200</v>
+      <c r="G156" s="22">
+        <v>120</v>
       </c>
       <c r="H156" s="22">
         <v>1000</v>
@@ -9445,14 +9363,14 @@
       <c r="F158" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G158" s="24">
-        <v>200</v>
-      </c>
-      <c r="H158" s="24">
-        <v>200</v>
-      </c>
-      <c r="I158" s="24">
-        <v>200</v>
+      <c r="G158" s="22">
+        <v>218</v>
+      </c>
+      <c r="H158" s="22">
+        <v>219</v>
+      </c>
+      <c r="I158" s="22">
+        <v>140</v>
       </c>
       <c r="J158" s="22">
         <v>1000</v>
@@ -9495,11 +9413,11 @@
       <c r="F159" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G159" s="24">
-        <v>200</v>
-      </c>
-      <c r="H159" s="24">
-        <v>200</v>
+      <c r="G159" s="22">
+        <v>184</v>
+      </c>
+      <c r="H159" s="22">
+        <v>185</v>
       </c>
       <c r="I159" s="22">
         <v>1000</v>
@@ -9545,17 +9463,17 @@
       <c r="F160" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G160" s="24">
-        <v>200</v>
-      </c>
-      <c r="H160" s="24">
-        <v>200</v>
-      </c>
-      <c r="I160" s="24">
-        <v>200</v>
-      </c>
-      <c r="J160" s="24">
-        <v>200</v>
+      <c r="G160" s="22">
+        <v>109</v>
+      </c>
+      <c r="H160" s="22">
+        <v>109</v>
+      </c>
+      <c r="I160" s="22">
+        <v>63</v>
+      </c>
+      <c r="J160" s="22">
+        <v>64</v>
       </c>
       <c r="K160" s="22">
         <v>1000</v>
@@ -9595,14 +9513,14 @@
       <c r="F161" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G161" s="25">
-        <v>200</v>
-      </c>
-      <c r="H161" s="25">
-        <v>200</v>
-      </c>
-      <c r="I161" s="25">
-        <v>200</v>
+      <c r="G161" s="21">
+        <v>172</v>
+      </c>
+      <c r="H161" s="21">
+        <v>173</v>
+      </c>
+      <c r="I161" s="21">
+        <v>174</v>
       </c>
       <c r="J161" s="21">
         <v>1000</v>
@@ -9645,11 +9563,11 @@
       <c r="F162" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G162" s="25">
-        <v>200</v>
-      </c>
-      <c r="H162" s="25">
-        <v>200</v>
+      <c r="G162" s="21">
+        <v>195</v>
+      </c>
+      <c r="H162" s="21">
+        <v>196</v>
       </c>
       <c r="I162" s="21">
         <v>1000</v>
@@ -9695,17 +9613,17 @@
       <c r="F163" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G163" s="25">
-        <v>200</v>
-      </c>
-      <c r="H163" s="25">
-        <v>200</v>
-      </c>
-      <c r="I163" s="25">
-        <v>200</v>
-      </c>
-      <c r="J163" s="25">
-        <v>200</v>
+      <c r="G163" s="21">
+        <v>28</v>
+      </c>
+      <c r="H163" s="21">
+        <v>29</v>
+      </c>
+      <c r="I163" s="21">
+        <v>20</v>
+      </c>
+      <c r="J163" s="21">
+        <v>21</v>
       </c>
       <c r="K163" s="21">
         <v>1000</v>
@@ -9745,8 +9663,8 @@
       <c r="F164" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G164" s="25">
-        <v>200</v>
+      <c r="G164" s="21">
+        <v>38</v>
       </c>
       <c r="H164" s="21">
         <v>1000</v>
@@ -9795,8 +9713,8 @@
       <c r="F165" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G165" s="25">
-        <v>200</v>
+      <c r="G165" s="21">
+        <v>9</v>
       </c>
       <c r="H165" s="21">
         <v>1000</v>
@@ -9895,17 +9813,17 @@
       <c r="F167" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G167" s="25">
-        <v>200</v>
-      </c>
-      <c r="H167" s="25">
-        <v>200</v>
-      </c>
-      <c r="I167" s="25">
-        <v>200</v>
-      </c>
-      <c r="J167" s="25">
-        <v>200</v>
+      <c r="G167" s="21">
+        <v>150</v>
+      </c>
+      <c r="H167" s="21">
+        <v>151</v>
+      </c>
+      <c r="I167" s="21">
+        <v>152</v>
+      </c>
+      <c r="J167" s="21">
+        <v>160</v>
       </c>
       <c r="K167" s="21">
         <v>1000</v>
@@ -9945,8 +9863,8 @@
       <c r="F168" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G168" s="25">
-        <v>200</v>
+      <c r="G168" s="21">
+        <v>75</v>
       </c>
       <c r="H168" s="21">
         <v>1000</v>
@@ -9995,8 +9913,8 @@
       <c r="F169" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G169" s="25">
-        <v>200</v>
+      <c r="G169" s="21">
+        <v>95</v>
       </c>
       <c r="H169" s="21">
         <v>1000</v>
@@ -10095,8 +10013,8 @@
       <c r="F171" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G171" s="24">
-        <v>200</v>
+      <c r="G171" s="22">
+        <v>43</v>
       </c>
       <c r="H171" s="22">
         <v>1000</v>
@@ -10145,17 +10063,17 @@
       <c r="F172" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G172" s="24">
-        <v>200</v>
-      </c>
-      <c r="H172" s="24">
-        <v>200</v>
-      </c>
-      <c r="I172" s="24">
-        <v>200</v>
-      </c>
-      <c r="J172" s="24">
-        <v>200</v>
+      <c r="G172" s="22">
+        <v>193</v>
+      </c>
+      <c r="H172" s="22">
+        <v>194</v>
+      </c>
+      <c r="I172" s="22">
+        <v>195</v>
+      </c>
+      <c r="J172" s="22">
+        <v>196</v>
       </c>
       <c r="K172" s="22">
         <v>1000</v>
@@ -10195,14 +10113,14 @@
       <c r="F173" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G173" s="24">
-        <v>200</v>
-      </c>
-      <c r="H173" s="24">
-        <v>200</v>
-      </c>
-      <c r="I173" s="24">
-        <v>200</v>
+      <c r="G173" s="22">
+        <v>171</v>
+      </c>
+      <c r="H173" s="22">
+        <v>172</v>
+      </c>
+      <c r="I173" s="22">
+        <v>71</v>
       </c>
       <c r="J173" s="22">
         <v>1000</v>
@@ -10245,17 +10163,17 @@
       <c r="F174" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G174" s="24">
-        <v>200</v>
-      </c>
-      <c r="H174" s="24">
-        <v>200</v>
-      </c>
-      <c r="I174" s="24">
-        <v>200</v>
-      </c>
-      <c r="J174" s="24">
-        <v>200</v>
+      <c r="G174" s="22">
+        <v>159</v>
+      </c>
+      <c r="H174" s="22">
+        <v>160</v>
+      </c>
+      <c r="I174" s="22">
+        <v>161</v>
+      </c>
+      <c r="J174" s="22">
+        <v>108</v>
       </c>
       <c r="K174" s="22">
         <v>1000</v>
@@ -10295,11 +10213,11 @@
       <c r="F175" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G175" s="24">
-        <v>200</v>
-      </c>
-      <c r="H175" s="24">
-        <v>200</v>
+      <c r="G175" s="22">
+        <v>129</v>
+      </c>
+      <c r="H175" s="22">
+        <v>130</v>
       </c>
       <c r="I175" s="22">
         <v>1000</v>
@@ -10345,23 +10263,23 @@
       <c r="F176" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G176" s="24">
-        <v>200</v>
-      </c>
-      <c r="H176" s="24">
-        <v>200</v>
-      </c>
-      <c r="I176" s="24">
-        <v>200</v>
-      </c>
-      <c r="J176" s="24">
-        <v>200</v>
-      </c>
-      <c r="K176" s="24">
-        <v>200</v>
-      </c>
-      <c r="L176" s="24">
-        <v>200</v>
+      <c r="G176" s="22">
+        <v>118</v>
+      </c>
+      <c r="H176" s="22">
+        <v>119</v>
+      </c>
+      <c r="I176" s="22">
+        <v>120</v>
+      </c>
+      <c r="J176" s="22">
+        <v>29</v>
+      </c>
+      <c r="K176" s="22">
+        <v>30</v>
+      </c>
+      <c r="L176" s="22">
+        <v>31</v>
       </c>
       <c r="M176" s="22">
         <v>1000</v>
@@ -10395,8 +10313,8 @@
       <c r="F177" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G177" s="24">
-        <v>200</v>
+      <c r="G177" s="22">
+        <v>153</v>
       </c>
       <c r="H177" s="22">
         <v>1000</v>
@@ -10445,20 +10363,20 @@
       <c r="F178" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G178" s="24">
-        <v>200</v>
-      </c>
-      <c r="H178" s="24">
-        <v>200</v>
-      </c>
-      <c r="I178" s="24">
-        <v>200</v>
-      </c>
-      <c r="J178" s="24">
-        <v>200</v>
-      </c>
-      <c r="K178" s="24">
-        <v>200</v>
+      <c r="G178" s="22">
+        <v>216</v>
+      </c>
+      <c r="H178" s="22">
+        <v>217</v>
+      </c>
+      <c r="I178" s="22">
+        <v>16</v>
+      </c>
+      <c r="J178" s="22">
+        <v>17</v>
+      </c>
+      <c r="K178" s="22">
+        <v>18</v>
       </c>
       <c r="L178" s="22">
         <v>1000</v>
@@ -10495,11 +10413,11 @@
       <c r="F179" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G179" s="24">
-        <v>200</v>
-      </c>
-      <c r="H179" s="24">
-        <v>200</v>
+      <c r="G179" s="22">
+        <v>181</v>
+      </c>
+      <c r="H179" s="22">
+        <v>7</v>
       </c>
       <c r="I179" s="22">
         <v>1000</v>
@@ -10545,20 +10463,20 @@
       <c r="F180" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G180" s="24">
-        <v>200</v>
-      </c>
-      <c r="H180" s="24">
-        <v>200</v>
-      </c>
-      <c r="I180" s="24">
-        <v>200</v>
-      </c>
-      <c r="J180" s="24">
-        <v>200</v>
-      </c>
-      <c r="K180" s="24">
-        <v>200</v>
+      <c r="G180" s="22">
+        <v>137</v>
+      </c>
+      <c r="H180" s="22">
+        <v>138</v>
+      </c>
+      <c r="I180" s="22">
+        <v>139</v>
+      </c>
+      <c r="J180" s="22">
+        <v>140</v>
+      </c>
+      <c r="K180" s="22">
+        <v>87</v>
       </c>
       <c r="L180" s="22">
         <v>1000</v>
@@ -10595,14 +10513,14 @@
       <c r="F181" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G181" s="25">
-        <v>200</v>
-      </c>
-      <c r="H181" s="25">
-        <v>200</v>
-      </c>
-      <c r="I181" s="25">
-        <v>200</v>
+      <c r="G181" s="21">
+        <v>10</v>
+      </c>
+      <c r="H181" s="21">
+        <v>163</v>
+      </c>
+      <c r="I181" s="21">
+        <v>164</v>
       </c>
       <c r="J181" s="21">
         <v>1000</v>
@@ -10645,14 +10563,14 @@
       <c r="F182" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G182" s="25">
-        <v>200</v>
-      </c>
-      <c r="H182" s="25">
-        <v>200</v>
-      </c>
-      <c r="I182" s="25">
-        <v>200</v>
+      <c r="G182" s="21">
+        <v>16</v>
+      </c>
+      <c r="H182" s="21">
+        <v>17</v>
+      </c>
+      <c r="I182" s="21">
+        <v>174</v>
       </c>
       <c r="J182" s="21">
         <v>1000</v>
@@ -10695,23 +10613,23 @@
       <c r="F183" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G183" s="25">
-        <v>200</v>
-      </c>
-      <c r="H183" s="25">
-        <v>200</v>
-      </c>
-      <c r="I183" s="25">
-        <v>200</v>
-      </c>
-      <c r="J183" s="25">
-        <v>200</v>
-      </c>
-      <c r="K183" s="25">
-        <v>200</v>
-      </c>
-      <c r="L183" s="25">
-        <v>200</v>
+      <c r="G183" s="21">
+        <v>29</v>
+      </c>
+      <c r="H183" s="21">
+        <v>30</v>
+      </c>
+      <c r="I183" s="21">
+        <v>31</v>
+      </c>
+      <c r="J183" s="21">
+        <v>214</v>
+      </c>
+      <c r="K183" s="21">
+        <v>215</v>
+      </c>
+      <c r="L183" s="21">
+        <v>216</v>
       </c>
       <c r="M183" s="21">
         <v>1000</v>
@@ -10745,14 +10663,14 @@
       <c r="F184" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G184" s="25">
-        <v>200</v>
-      </c>
-      <c r="H184" s="25">
-        <v>200</v>
-      </c>
-      <c r="I184" s="25">
-        <v>200</v>
+      <c r="G184" s="21">
+        <v>40</v>
+      </c>
+      <c r="H184" s="21">
+        <v>41</v>
+      </c>
+      <c r="I184" s="21">
+        <v>119</v>
       </c>
       <c r="J184" s="21">
         <v>1000</v>
@@ -10795,11 +10713,11 @@
       <c r="F185" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G185" s="25">
-        <v>200</v>
-      </c>
-      <c r="H185" s="25">
-        <v>200</v>
+      <c r="G185" s="21">
+        <v>50</v>
+      </c>
+      <c r="H185" s="21">
+        <v>51</v>
       </c>
       <c r="I185" s="21">
         <v>1000</v>
@@ -10845,8 +10763,8 @@
       <c r="F186" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G186" s="25">
-        <v>200</v>
+      <c r="G186" s="21">
+        <v>63</v>
       </c>
       <c r="H186" s="21">
         <v>1000</v>
@@ -10945,8 +10863,8 @@
       <c r="F188" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G188" s="25">
-        <v>200</v>
+      <c r="G188" s="21">
+        <v>207</v>
       </c>
       <c r="H188" s="21">
         <v>1000</v>
@@ -10995,14 +10913,14 @@
       <c r="F189" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G189" s="25">
-        <v>200</v>
-      </c>
-      <c r="H189" s="25">
-        <v>200</v>
-      </c>
-      <c r="I189" s="25">
-        <v>200</v>
+      <c r="G189" s="21">
+        <v>97</v>
+      </c>
+      <c r="H189" s="21">
+        <v>193</v>
+      </c>
+      <c r="I189" s="21">
+        <v>194</v>
       </c>
       <c r="J189" s="21">
         <v>1000</v>
@@ -11045,8 +10963,8 @@
       <c r="F190" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G190" s="25">
-        <v>200</v>
+      <c r="G190" s="21">
+        <v>104</v>
       </c>
       <c r="H190" s="21">
         <v>1000</v>
@@ -11095,17 +11013,17 @@
       <c r="F191" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G191" s="24">
-        <v>200</v>
-      </c>
-      <c r="H191" s="24">
-        <v>200</v>
-      </c>
-      <c r="I191" s="24">
-        <v>200</v>
-      </c>
-      <c r="J191" s="24">
-        <v>200</v>
+      <c r="G191" s="22">
+        <v>203</v>
+      </c>
+      <c r="H191" s="22">
+        <v>204</v>
+      </c>
+      <c r="I191" s="22">
+        <v>205</v>
+      </c>
+      <c r="J191" s="22">
+        <v>98</v>
       </c>
       <c r="K191" s="22">
         <v>1000</v>
@@ -11145,20 +11063,20 @@
       <c r="F192" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G192" s="24">
-        <v>200</v>
-      </c>
-      <c r="H192" s="24">
-        <v>200</v>
-      </c>
-      <c r="I192" s="24">
-        <v>200</v>
-      </c>
-      <c r="J192" s="24">
-        <v>200</v>
-      </c>
-      <c r="K192" s="24">
-        <v>200</v>
+      <c r="G192" s="22">
+        <v>193</v>
+      </c>
+      <c r="H192" s="22">
+        <v>194</v>
+      </c>
+      <c r="I192" s="22">
+        <v>195</v>
+      </c>
+      <c r="J192" s="22">
+        <v>196</v>
+      </c>
+      <c r="K192" s="22">
+        <v>86</v>
       </c>
       <c r="L192" s="22">
         <v>1000</v>
@@ -11195,8 +11113,8 @@
       <c r="F193" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G193" s="24">
-        <v>200</v>
+      <c r="G193" s="22">
+        <v>174</v>
       </c>
       <c r="H193" s="22">
         <v>1000</v>
@@ -11245,8 +11163,8 @@
       <c r="F194" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G194" s="24">
-        <v>200</v>
+      <c r="G194" s="22">
+        <v>159</v>
       </c>
       <c r="H194" s="22">
         <v>1000</v>
@@ -11295,17 +11213,17 @@
       <c r="F195" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G195" s="24">
-        <v>200</v>
-      </c>
-      <c r="H195" s="24">
-        <v>200</v>
-      </c>
-      <c r="I195" s="24">
-        <v>200</v>
-      </c>
-      <c r="J195" s="24">
-        <v>200</v>
+      <c r="G195" s="22">
+        <v>130</v>
+      </c>
+      <c r="H195" s="22">
+        <v>131</v>
+      </c>
+      <c r="I195" s="22">
+        <v>16</v>
+      </c>
+      <c r="J195" s="22">
+        <v>17</v>
       </c>
       <c r="K195" s="22">
         <v>1000</v>
@@ -11345,14 +11263,14 @@
       <c r="F196" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G196" s="24">
-        <v>200</v>
-      </c>
-      <c r="H196" s="24">
-        <v>200</v>
-      </c>
-      <c r="I196" s="24">
-        <v>200</v>
+      <c r="G196" s="22">
+        <v>118</v>
+      </c>
+      <c r="H196" s="22">
+        <v>119</v>
+      </c>
+      <c r="I196" s="22">
+        <v>120</v>
       </c>
       <c r="J196" s="22">
         <v>1000</v>
@@ -11395,14 +11313,14 @@
       <c r="F197" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G197" s="24">
-        <v>200</v>
-      </c>
-      <c r="H197" s="24">
-        <v>200</v>
-      </c>
-      <c r="I197" s="24">
-        <v>200</v>
+      <c r="G197" s="22">
+        <v>150</v>
+      </c>
+      <c r="H197" s="22">
+        <v>41</v>
+      </c>
+      <c r="I197" s="22">
+        <v>42</v>
       </c>
       <c r="J197" s="22">
         <v>1000</v>
@@ -11445,8 +11363,8 @@
       <c r="F198" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G198" s="24">
-        <v>200</v>
+      <c r="G198" s="22">
+        <v>218</v>
       </c>
       <c r="H198" s="22">
         <v>1000</v>
@@ -11495,8 +11413,8 @@
       <c r="F199" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G199" s="24">
-        <v>200</v>
+      <c r="G199" s="22">
+        <v>76</v>
       </c>
       <c r="H199" s="22">
         <v>1000</v>
@@ -11545,8 +11463,8 @@
       <c r="F200" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G200" s="24">
-        <v>200</v>
+      <c r="G200" s="22">
+        <v>141</v>
       </c>
       <c r="H200" s="22">
         <v>1000</v>
@@ -11595,20 +11513,20 @@
       <c r="F201" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G201" s="25">
-        <v>200</v>
-      </c>
-      <c r="H201" s="25">
-        <v>200</v>
-      </c>
-      <c r="I201" s="25">
-        <v>200</v>
-      </c>
-      <c r="J201" s="25">
-        <v>200</v>
-      </c>
-      <c r="K201" s="25">
-        <v>200</v>
+      <c r="G201" s="21">
+        <v>8</v>
+      </c>
+      <c r="H201" s="21">
+        <v>9</v>
+      </c>
+      <c r="I201" s="21">
+        <v>139</v>
+      </c>
+      <c r="J201" s="21">
+        <v>140</v>
+      </c>
+      <c r="K201" s="21">
+        <v>141</v>
       </c>
       <c r="L201" s="21">
         <v>1000</v>
@@ -11645,8 +11563,8 @@
       <c r="F202" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G202" s="25">
-        <v>200</v>
+      <c r="G202" s="21">
+        <v>17</v>
       </c>
       <c r="H202" s="21">
         <v>1000</v>
@@ -11695,8 +11613,8 @@
       <c r="F203" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G203" s="25">
-        <v>200</v>
+      <c r="G203" s="21">
+        <v>195</v>
       </c>
       <c r="H203" s="21">
         <v>1000</v>
@@ -11745,14 +11663,14 @@
       <c r="F204" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G204" s="25">
-        <v>200</v>
-      </c>
-      <c r="H204" s="25">
-        <v>200</v>
-      </c>
-      <c r="I204" s="25">
-        <v>200</v>
+      <c r="G204" s="21">
+        <v>40</v>
+      </c>
+      <c r="H204" s="21">
+        <v>41</v>
+      </c>
+      <c r="I204" s="21">
+        <v>42</v>
       </c>
       <c r="J204" s="21">
         <v>1000</v>
@@ -11795,11 +11713,11 @@
       <c r="F205" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G205" s="25">
-        <v>200</v>
-      </c>
-      <c r="H205" s="25">
-        <v>200</v>
+      <c r="G205" s="21">
+        <v>51</v>
+      </c>
+      <c r="H205" s="21">
+        <v>151</v>
       </c>
       <c r="I205" s="21">
         <v>1000</v>
@@ -11845,8 +11763,8 @@
       <c r="F206" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G206" s="25">
-        <v>200</v>
+      <c r="G206" s="21">
+        <v>207</v>
       </c>
       <c r="H206" s="21">
         <v>1000</v>
@@ -11895,14 +11813,14 @@
       <c r="F207" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G207" s="25">
-        <v>200</v>
-      </c>
-      <c r="H207" s="25">
-        <v>200</v>
-      </c>
-      <c r="I207" s="25">
-        <v>200</v>
+      <c r="G207" s="21">
+        <v>73</v>
+      </c>
+      <c r="H207" s="21">
+        <v>74</v>
+      </c>
+      <c r="I207" s="21">
+        <v>75</v>
       </c>
       <c r="J207" s="21">
         <v>1000</v>
@@ -11945,14 +11863,14 @@
       <c r="F208" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G208" s="25">
-        <v>200</v>
-      </c>
-      <c r="H208" s="25">
-        <v>200</v>
-      </c>
-      <c r="I208" s="25">
-        <v>200</v>
+      <c r="G208" s="21">
+        <v>85</v>
+      </c>
+      <c r="H208" s="21">
+        <v>86</v>
+      </c>
+      <c r="I208" s="21">
+        <v>171</v>
       </c>
       <c r="J208" s="21">
         <v>1000</v>
@@ -11995,11 +11913,11 @@
       <c r="F209" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G209" s="25">
-        <v>200</v>
-      </c>
-      <c r="H209" s="25">
-        <v>200</v>
+      <c r="G209" s="21">
+        <v>98</v>
+      </c>
+      <c r="H209" s="21">
+        <v>159</v>
       </c>
       <c r="I209" s="21">
         <v>1000</v>
@@ -12045,14 +11963,14 @@
       <c r="F210" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G210" s="25">
-        <v>200</v>
-      </c>
-      <c r="H210" s="25">
-        <v>200</v>
-      </c>
-      <c r="I210" s="25">
-        <v>200</v>
+      <c r="G210" s="21">
+        <v>107</v>
+      </c>
+      <c r="H210" s="21">
+        <v>128</v>
+      </c>
+      <c r="I210" s="21">
+        <v>129</v>
       </c>
       <c r="J210" s="21">
         <v>1000</v>
@@ -12086,17 +12004,17 @@
       <c r="C211" s="16">
         <v>1</v>
       </c>
-      <c r="D211" s="26">
+      <c r="D211" s="24">
         <v>0</v>
       </c>
       <c r="E211" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F211" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G211" s="24">
-        <v>200</v>
+        <v>20</v>
+      </c>
+      <c r="G211" s="22">
+        <v>207</v>
       </c>
       <c r="H211" s="22">
         <v>1000</v>
@@ -12136,29 +12054,29 @@
       <c r="C212" s="16">
         <v>5</v>
       </c>
-      <c r="D212" s="26">
+      <c r="D212" s="24">
         <v>0</v>
       </c>
       <c r="E212" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F212" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G212" s="24">
-        <v>200</v>
-      </c>
-      <c r="H212" s="24">
-        <v>200</v>
-      </c>
-      <c r="I212" s="24">
-        <v>200</v>
-      </c>
-      <c r="J212" s="24">
-        <v>200</v>
-      </c>
-      <c r="K212" s="24">
-        <v>200</v>
+        <v>20</v>
+      </c>
+      <c r="G212" s="22">
+        <v>192</v>
+      </c>
+      <c r="H212" s="22">
+        <v>193</v>
+      </c>
+      <c r="I212" s="22">
+        <v>194</v>
+      </c>
+      <c r="J212" s="22">
+        <v>195</v>
+      </c>
+      <c r="K212" s="22">
+        <v>196</v>
       </c>
       <c r="L212" s="22">
         <v>1000</v>
@@ -12186,23 +12104,23 @@
       <c r="C213" s="16">
         <v>3</v>
       </c>
-      <c r="D213" s="26">
+      <c r="D213" s="24">
         <v>0</v>
       </c>
       <c r="E213" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F213" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G213" s="24">
-        <v>200</v>
-      </c>
-      <c r="H213" s="24">
-        <v>200</v>
-      </c>
-      <c r="I213" s="24">
-        <v>200</v>
+        <v>20</v>
+      </c>
+      <c r="G213" s="22">
+        <v>29</v>
+      </c>
+      <c r="H213" s="22">
+        <v>30</v>
+      </c>
+      <c r="I213" s="22">
+        <v>31</v>
       </c>
       <c r="J213" s="22">
         <v>1000</v>
@@ -12236,17 +12154,17 @@
       <c r="C214" s="16">
         <v>0</v>
       </c>
-      <c r="D214" s="26">
+      <c r="D214" s="24">
         <v>1</v>
       </c>
       <c r="E214" s="10" t="s">
         <v>0</v>
       </c>
       <c r="F214" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G214" s="24">
-        <v>200</v>
+        <v>20</v>
+      </c>
+      <c r="G214" s="22">
+        <v>38</v>
       </c>
       <c r="H214" s="22">
         <v>1000</v>
@@ -12286,14 +12204,14 @@
       <c r="C215" s="16">
         <v>0</v>
       </c>
-      <c r="D215" s="26">
+      <c r="D215" s="24">
         <v>0</v>
       </c>
       <c r="E215" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F215" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G215" s="22">
         <v>1000</v>
@@ -12336,23 +12254,23 @@
       <c r="C216" s="16">
         <v>3</v>
       </c>
-      <c r="D216" s="26">
+      <c r="D216" s="24">
         <v>0</v>
       </c>
       <c r="E216" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F216" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G216" s="24">
-        <v>200</v>
-      </c>
-      <c r="H216" s="24">
-        <v>200</v>
-      </c>
-      <c r="I216" s="24">
-        <v>200</v>
+        <v>20</v>
+      </c>
+      <c r="G216" s="22">
+        <v>118</v>
+      </c>
+      <c r="H216" s="22">
+        <v>119</v>
+      </c>
+      <c r="I216" s="22">
+        <v>120</v>
       </c>
       <c r="J216" s="22">
         <v>1000</v>
@@ -12386,17 +12304,17 @@
       <c r="C217" s="16">
         <v>0</v>
       </c>
-      <c r="D217" s="26">
+      <c r="D217" s="24">
         <v>1</v>
       </c>
       <c r="E217" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F217" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G217" s="24">
-        <v>200</v>
+        <v>20</v>
+      </c>
+      <c r="G217" s="22">
+        <v>74</v>
       </c>
       <c r="H217" s="22">
         <v>1000</v>
@@ -12436,20 +12354,20 @@
       <c r="C218" s="16">
         <v>1</v>
       </c>
-      <c r="D218" s="26">
+      <c r="D218" s="24">
         <v>1</v>
       </c>
       <c r="E218" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F218" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G218" s="24">
-        <v>200</v>
-      </c>
-      <c r="H218" s="24">
-        <v>200</v>
+        <v>20</v>
+      </c>
+      <c r="G218" s="22">
+        <v>218</v>
+      </c>
+      <c r="H218" s="22">
+        <v>96</v>
       </c>
       <c r="I218" s="22">
         <v>1000</v>
@@ -12486,17 +12404,17 @@
       <c r="C219" s="16">
         <v>1</v>
       </c>
-      <c r="D219" s="26">
+      <c r="D219" s="24">
         <v>0</v>
       </c>
       <c r="E219" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F219" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G219" s="24">
-        <v>200</v>
+        <v>20</v>
+      </c>
+      <c r="G219" s="22">
+        <v>186</v>
       </c>
       <c r="H219" s="22">
         <v>1000</v>
@@ -12536,17 +12454,17 @@
       <c r="C220" s="16">
         <v>0</v>
       </c>
-      <c r="D220" s="26">
+      <c r="D220" s="24">
         <v>1</v>
       </c>
       <c r="E220" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F220" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G220" s="24">
-        <v>200</v>
+        <v>20</v>
+      </c>
+      <c r="G220" s="22">
+        <v>9</v>
       </c>
       <c r="H220" s="22">
         <v>1000</v>
@@ -20578,657 +20496,657 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B380">
-    <cfRule type="cellIs" dxfId="142" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="239" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F380">
-    <cfRule type="cellIs" dxfId="141" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="237" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E380">
-    <cfRule type="cellIs" dxfId="140" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="236" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:P1">
-    <cfRule type="cellIs" dxfId="139" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="235" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:J3">
-    <cfRule type="cellIs" dxfId="138" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="234" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:P20">
-    <cfRule type="cellIs" dxfId="137" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="232" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21:P30">
-    <cfRule type="cellIs" dxfId="136" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="231" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:P30">
-    <cfRule type="cellIs" dxfId="135" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="230" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:K4">
-    <cfRule type="cellIs" dxfId="134" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="176" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:J5">
-    <cfRule type="cellIs" dxfId="133" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="175" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:P2">
-    <cfRule type="cellIs" dxfId="132" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="122" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:P3">
-    <cfRule type="cellIs" dxfId="131" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="121" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:P4">
-    <cfRule type="cellIs" dxfId="130" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="120" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:P5">
-    <cfRule type="cellIs" dxfId="129" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="119" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:P10">
-    <cfRule type="cellIs" dxfId="128" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="118" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:P40">
-    <cfRule type="cellIs" dxfId="127" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="117" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41:P50">
-    <cfRule type="cellIs" dxfId="126" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="116" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:P50">
-    <cfRule type="cellIs" dxfId="125" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="115" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51:P60">
-    <cfRule type="cellIs" dxfId="124" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="114" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G61:P70">
-    <cfRule type="cellIs" dxfId="123" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="113" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62:P70">
-    <cfRule type="cellIs" dxfId="122" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="112" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G71:P80">
-    <cfRule type="cellIs" dxfId="121" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="111" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81:P90">
-    <cfRule type="cellIs" dxfId="120" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="110" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82:P90">
-    <cfRule type="cellIs" dxfId="119" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="109" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91:P100">
-    <cfRule type="cellIs" dxfId="118" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="108" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G101:P110">
-    <cfRule type="cellIs" dxfId="117" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="107" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102:P110">
-    <cfRule type="cellIs" dxfId="116" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="106" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G111:P120">
-    <cfRule type="cellIs" dxfId="115" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="105" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G121:P130">
-    <cfRule type="cellIs" dxfId="114" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="104" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G122:P130">
-    <cfRule type="cellIs" dxfId="113" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="103" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G131:P140">
-    <cfRule type="cellIs" dxfId="112" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="102" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G141:P150">
-    <cfRule type="cellIs" dxfId="111" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="101" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G142:P150">
-    <cfRule type="cellIs" dxfId="110" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="100" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G151:P160">
-    <cfRule type="cellIs" dxfId="109" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="99" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G161:P170">
-    <cfRule type="cellIs" dxfId="108" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="98" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G162:P170">
-    <cfRule type="cellIs" dxfId="107" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="97" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L180:P180 H171:P171 K172:P172 J173:P173 K174:P174 I175:P175 M176:P176 H177:P177 L178:P178 I179:P179">
-    <cfRule type="cellIs" dxfId="106" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="96" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:P187 J181:P182 M183:P183 J184:P184 I185:P185 H186:P186 H190:P190 H188:P188 J189:P189">
-    <cfRule type="cellIs" dxfId="105" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="95" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:P187 J182:P182 M183:P183 J184:P184 I185:P185 H186:P186 H190:P190 H188:P188 J189:P189">
-    <cfRule type="cellIs" dxfId="104" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="94" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K191:P191 L192:P192 H193:P194 K195:P195 J196:P197 H198:P200">
-    <cfRule type="cellIs" dxfId="103" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="93" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J210:P210 L201:P201 H202:P203 J204:P204 I205:P205 H206:P206 J207:P208 I209:P209">
-    <cfRule type="cellIs" dxfId="102" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="92" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J210:P210 H202:P203 J204:P204 I205:P205 H206:P206 J207:P208 I209:P209">
-    <cfRule type="cellIs" dxfId="101" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G215:P215 H211:P211 L212:P212 J213:P213 H214:P214 J216:P216 H217:P217 I218:P218 H219:P220">
-    <cfRule type="cellIs" dxfId="100" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="90" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G221:P230">
-    <cfRule type="cellIs" dxfId="99" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="89" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G222:P230">
-    <cfRule type="cellIs" dxfId="98" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="88" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G231:P240">
-    <cfRule type="cellIs" dxfId="97" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="87" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G241:P250">
-    <cfRule type="cellIs" dxfId="96" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="86" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G242:P250">
-    <cfRule type="cellIs" dxfId="95" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="85" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G251:P260">
-    <cfRule type="cellIs" dxfId="94" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="84" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G261:P270">
-    <cfRule type="cellIs" dxfId="93" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="83" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G262:P270">
-    <cfRule type="cellIs" dxfId="92" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G271:P280">
-    <cfRule type="cellIs" dxfId="91" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="81" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G281:P290">
-    <cfRule type="cellIs" dxfId="90" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="80" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G282:P290">
-    <cfRule type="cellIs" dxfId="89" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="79" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G291:P300">
-    <cfRule type="cellIs" dxfId="88" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="78" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G301:P310">
-    <cfRule type="cellIs" dxfId="87" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G302:P310">
-    <cfRule type="cellIs" dxfId="86" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="76" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G311:P320">
-    <cfRule type="cellIs" dxfId="85" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="75" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G321:P330">
-    <cfRule type="cellIs" dxfId="84" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="74" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G322:P330">
-    <cfRule type="cellIs" dxfId="83" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="73" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G331:P340">
-    <cfRule type="cellIs" dxfId="82" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="72" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G341:P350">
-    <cfRule type="cellIs" dxfId="81" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G342:P350">
-    <cfRule type="cellIs" dxfId="80" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G351:P360">
-    <cfRule type="cellIs" dxfId="79" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="69" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G361:P370">
-    <cfRule type="cellIs" dxfId="78" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="68" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G362:P370">
-    <cfRule type="cellIs" dxfId="77" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="67" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G371:P380">
-    <cfRule type="cellIs" dxfId="76" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G171">
-    <cfRule type="cellIs" dxfId="75" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="65" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G172:J172">
-    <cfRule type="cellIs" dxfId="74" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="64" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G173:I173">
-    <cfRule type="cellIs" dxfId="73" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G174:J174">
-    <cfRule type="cellIs" dxfId="72" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="62" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G175:H175">
-    <cfRule type="cellIs" dxfId="71" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G176:L176">
-    <cfRule type="cellIs" dxfId="70" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="60" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G177">
-    <cfRule type="cellIs" dxfId="69" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G178:K178">
-    <cfRule type="cellIs" dxfId="68" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G179:H179">
-    <cfRule type="cellIs" dxfId="67" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G180:K180">
-    <cfRule type="cellIs" dxfId="66" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="56" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G181:I181">
-    <cfRule type="cellIs" dxfId="65" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G181:I181">
-    <cfRule type="cellIs" dxfId="64" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G182:I182">
-    <cfRule type="cellIs" dxfId="63" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G182:I182">
-    <cfRule type="cellIs" dxfId="62" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G183:L183">
-    <cfRule type="cellIs" dxfId="61" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G183:L183">
-    <cfRule type="cellIs" dxfId="60" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G184:I184">
-    <cfRule type="cellIs" dxfId="59" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G184:I184">
-    <cfRule type="cellIs" dxfId="58" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:H185">
-    <cfRule type="cellIs" dxfId="57" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:H185">
-    <cfRule type="cellIs" dxfId="56" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G186">
-    <cfRule type="cellIs" dxfId="55" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G186">
-    <cfRule type="cellIs" dxfId="54" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="44" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188">
-    <cfRule type="cellIs" dxfId="53" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188">
-    <cfRule type="cellIs" dxfId="52" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G189:I189">
-    <cfRule type="cellIs" dxfId="51" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G189:I189">
-    <cfRule type="cellIs" dxfId="50" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190">
-    <cfRule type="cellIs" dxfId="49" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190">
-    <cfRule type="cellIs" dxfId="48" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G191:J191">
-    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G192:K192">
-    <cfRule type="cellIs" dxfId="46" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G193:G194">
-    <cfRule type="cellIs" dxfId="45" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G195:J195">
-    <cfRule type="cellIs" dxfId="44" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G196:I196">
-    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G197:I197">
-    <cfRule type="cellIs" dxfId="42" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G198">
-    <cfRule type="cellIs" dxfId="41" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G199:G200">
-    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:K201">
-    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:K201">
-    <cfRule type="cellIs" dxfId="38" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202">
-    <cfRule type="cellIs" dxfId="37" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202">
-    <cfRule type="cellIs" dxfId="36" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203">
-    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203">
-    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G204:I204">
-    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G204:I204">
-    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G205:H205">
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G205:H205">
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G206">
-    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G206">
-    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:I207">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:I207">
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G208:I208">
-    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G208:I208">
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G209:H209">
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G209:H209">
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G210:I210">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G210:I210">
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G211">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G212:K212">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G213:I213">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G214">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G216:I216">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G217">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G218:H218">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G219">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adequações para ficar mais orientado a objetos.
</commit_message>
<xml_diff>
--- a/brasileirao/src/arquivos/partidas.xlsx
+++ b/brasileirao/src/arquivos/partidas.xlsx
@@ -273,14 +273,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="133">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="132">
     <dxf>
       <font>
         <b/>
@@ -1483,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F211" sqref="F211"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G151" sqref="G151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8764,13 +8757,13 @@
         <v>20</v>
       </c>
       <c r="G146" s="21">
-        <v>1000</v>
+        <v>63</v>
       </c>
       <c r="H146" s="21">
-        <v>1000</v>
+        <v>7</v>
       </c>
       <c r="I146" s="21">
-        <v>1000</v>
+        <v>8</v>
       </c>
       <c r="J146" s="21">
         <v>1000</v>
@@ -8814,10 +8807,10 @@
         <v>20</v>
       </c>
       <c r="G147" s="21">
-        <v>1000</v>
+        <v>151</v>
       </c>
       <c r="H147" s="21">
-        <v>1000</v>
+        <v>118</v>
       </c>
       <c r="I147" s="21">
         <v>1000</v>
@@ -8864,13 +8857,13 @@
         <v>20</v>
       </c>
       <c r="G148" s="21">
-        <v>1000</v>
+        <v>86</v>
       </c>
       <c r="H148" s="21">
-        <v>1000</v>
+        <v>26</v>
       </c>
       <c r="I148" s="21">
-        <v>1000</v>
+        <v>26</v>
       </c>
       <c r="J148" s="21">
         <v>1000</v>
@@ -8914,13 +8907,13 @@
         <v>20</v>
       </c>
       <c r="G149" s="21">
-        <v>1000</v>
+        <v>98</v>
       </c>
       <c r="H149" s="21">
-        <v>1000</v>
+        <v>186</v>
       </c>
       <c r="I149" s="21">
-        <v>1000</v>
+        <v>186</v>
       </c>
       <c r="J149" s="21">
         <v>1000</v>
@@ -8964,13 +8957,13 @@
         <v>20</v>
       </c>
       <c r="G150" s="21">
-        <v>1000</v>
+        <v>105</v>
       </c>
       <c r="H150" s="21">
-        <v>1000</v>
+        <v>105</v>
       </c>
       <c r="I150" s="21">
-        <v>1000</v>
+        <v>76</v>
       </c>
       <c r="J150" s="21">
         <v>1000</v>
@@ -20496,662 +20489,662 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B380">
-    <cfRule type="cellIs" dxfId="132" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="239" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F380">
-    <cfRule type="cellIs" dxfId="131" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="237" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E380">
-    <cfRule type="cellIs" dxfId="130" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="236" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:P1">
-    <cfRule type="cellIs" dxfId="129" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="235" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:J3">
-    <cfRule type="cellIs" dxfId="128" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="234" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:P20">
-    <cfRule type="cellIs" dxfId="127" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="232" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21:P30">
-    <cfRule type="cellIs" dxfId="126" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="231" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:P30">
-    <cfRule type="cellIs" dxfId="125" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="230" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:K4">
-    <cfRule type="cellIs" dxfId="124" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="176" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:J5">
-    <cfRule type="cellIs" dxfId="123" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="175" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:P2">
-    <cfRule type="cellIs" dxfId="122" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="122" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:P3">
-    <cfRule type="cellIs" dxfId="121" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="121" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:P4">
-    <cfRule type="cellIs" dxfId="120" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="120" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:P5">
-    <cfRule type="cellIs" dxfId="119" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="119" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:P10">
-    <cfRule type="cellIs" dxfId="118" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="118" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:P40">
-    <cfRule type="cellIs" dxfId="117" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="117" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41:P50">
-    <cfRule type="cellIs" dxfId="116" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="116" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:P50">
-    <cfRule type="cellIs" dxfId="115" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="115" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51:P60">
-    <cfRule type="cellIs" dxfId="114" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="114" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G61:P70">
-    <cfRule type="cellIs" dxfId="113" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="113" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62:P70">
-    <cfRule type="cellIs" dxfId="112" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="112" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G71:P80">
-    <cfRule type="cellIs" dxfId="111" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="111" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81:P90">
-    <cfRule type="cellIs" dxfId="110" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="110" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82:P90">
-    <cfRule type="cellIs" dxfId="109" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="109" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91:P100">
-    <cfRule type="cellIs" dxfId="108" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="108" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G101:P110">
-    <cfRule type="cellIs" dxfId="107" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="107" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102:P110">
-    <cfRule type="cellIs" dxfId="106" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="106" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G111:P120">
-    <cfRule type="cellIs" dxfId="105" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="105" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G121:P130">
-    <cfRule type="cellIs" dxfId="104" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="104" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G122:P130">
-    <cfRule type="cellIs" dxfId="103" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="103" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G131:P140">
-    <cfRule type="cellIs" dxfId="102" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="102" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G141:P150">
-    <cfRule type="cellIs" dxfId="101" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="101" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G142:P150">
-    <cfRule type="cellIs" dxfId="100" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="100" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G151:P160">
-    <cfRule type="cellIs" dxfId="99" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="99" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G161:P170">
-    <cfRule type="cellIs" dxfId="98" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="98" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G162:P170">
-    <cfRule type="cellIs" dxfId="97" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="97" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L180:P180 H171:P171 K172:P172 J173:P173 K174:P174 I175:P175 M176:P176 H177:P177 L178:P178 I179:P179">
-    <cfRule type="cellIs" dxfId="96" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="96" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:P187 J181:P182 M183:P183 J184:P184 I185:P185 H186:P186 H190:P190 H188:P188 J189:P189">
-    <cfRule type="cellIs" dxfId="95" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="95" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:P187 J182:P182 M183:P183 J184:P184 I185:P185 H186:P186 H190:P190 H188:P188 J189:P189">
-    <cfRule type="cellIs" dxfId="94" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="94" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K191:P191 L192:P192 H193:P194 K195:P195 J196:P197 H198:P200">
-    <cfRule type="cellIs" dxfId="93" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="93" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J210:P210 L201:P201 H202:P203 J204:P204 I205:P205 H206:P206 J207:P208 I209:P209">
-    <cfRule type="cellIs" dxfId="92" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="92" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J210:P210 H202:P203 J204:P204 I205:P205 H206:P206 J207:P208 I209:P209">
-    <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="91" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G215:P215 H211:P211 L212:P212 J213:P213 H214:P214 J216:P216 H217:P217 I218:P218 H219:P220">
-    <cfRule type="cellIs" dxfId="90" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="90" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G221:P230">
-    <cfRule type="cellIs" dxfId="89" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="89" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G222:P230">
-    <cfRule type="cellIs" dxfId="88" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="88" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G231:P240">
-    <cfRule type="cellIs" dxfId="87" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="87" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G241:P250">
-    <cfRule type="cellIs" dxfId="86" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="86" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G242:P250">
-    <cfRule type="cellIs" dxfId="85" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="85" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G251:P260">
-    <cfRule type="cellIs" dxfId="84" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="84" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G261:P270">
-    <cfRule type="cellIs" dxfId="83" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="83" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G262:P270">
-    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="82" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G271:P280">
-    <cfRule type="cellIs" dxfId="81" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="81" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G281:P290">
-    <cfRule type="cellIs" dxfId="80" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="80" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G282:P290">
-    <cfRule type="cellIs" dxfId="79" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G291:P300">
-    <cfRule type="cellIs" dxfId="78" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="78" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G301:P310">
-    <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="77" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G302:P310">
-    <cfRule type="cellIs" dxfId="76" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G311:P320">
-    <cfRule type="cellIs" dxfId="75" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G321:P330">
-    <cfRule type="cellIs" dxfId="74" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="74" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G322:P330">
-    <cfRule type="cellIs" dxfId="73" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="73" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G331:P340">
-    <cfRule type="cellIs" dxfId="72" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G341:P350">
-    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="71" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G342:P350">
-    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G351:P360">
-    <cfRule type="cellIs" dxfId="69" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="69" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G361:P370">
-    <cfRule type="cellIs" dxfId="68" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="68" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G362:P370">
-    <cfRule type="cellIs" dxfId="67" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G371:P380">
-    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="66" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G171">
-    <cfRule type="cellIs" dxfId="65" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G172:J172">
-    <cfRule type="cellIs" dxfId="64" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G173:I173">
-    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="63" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G174:J174">
-    <cfRule type="cellIs" dxfId="62" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G175:H175">
-    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G176:L176">
-    <cfRule type="cellIs" dxfId="60" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G177">
-    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G178:K178">
-    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G179:H179">
-    <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="57" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G180:K180">
-    <cfRule type="cellIs" dxfId="56" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G181:I181">
-    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G181:I181">
-    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G182:I182">
-    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G182:I182">
-    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G183:L183">
-    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G183:L183">
-    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G184:I184">
-    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G184:I184">
-    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:H185">
-    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:H185">
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G186">
-    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G186">
-    <cfRule type="cellIs" dxfId="44" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188">
-    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188">
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G189:I189">
-    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G189:I189">
-    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190">
-    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190">
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G191:J191">
-    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G192:K192">
-    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G193:G194">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G195:J195">
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G196:I196">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G197:I197">
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G198">
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G199:G200">
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:K201">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201:K201">
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G203">
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G204:I204">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G204:I204">
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G205:H205">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G205:H205">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G206">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G206">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:I207">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:I207">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G208:I208">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G208:I208">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G209:H209">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G209:H209">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G210:I210">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G210:I210">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G211">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G212:K212">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G213:I213">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G214">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G216:I216">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G217">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G218:H218">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G219">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G220">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>